<commit_message>
Updated excel sheet for week 3.
</commit_message>
<xml_diff>
--- a/2.2_P.CoB_Time_registration_for10.xlsx
+++ b/2.2_P.CoB_Time_registration_for10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Study\Current\Project Client On Board\ProjectClientOnBoardGitProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D6C6D0-203A-4C74-B7F2-C09CA50B71E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC007C88-88FE-4DAE-B74D-C4B55BEF6696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructie" sheetId="19" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>Manual</t>
   </si>
@@ -285,6 +285,21 @@
   </si>
   <si>
     <t>End sprint meeting, Team plan, Finalize Documents</t>
+  </si>
+  <si>
+    <t>Class one</t>
+  </si>
+  <si>
+    <t>Class two</t>
+  </si>
+  <si>
+    <t>Create new wireframes</t>
+  </si>
+  <si>
+    <t>Test case page, issue #9</t>
+  </si>
+  <si>
+    <t>Side menu, issue #97</t>
   </si>
 </sst>
 </file>
@@ -790,12 +805,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,6 +813,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,7 +1031,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1886,22 +1901,22 @@
                   <c:v>577.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>577.35</c:v>
+                  <c:v>566.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>577.35</c:v>
+                  <c:v>566.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>577.35</c:v>
+                  <c:v>566.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>577.35</c:v>
+                  <c:v>566.35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>577.35</c:v>
+                  <c:v>566.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>577.35</c:v>
+                  <c:v>566.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3450,32 +3465,32 @@
         <f>Total!$L$1</f>
         <v>Week 8</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -3625,16 +3640,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -3774,16 +3789,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -3923,16 +3938,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -4072,16 +4087,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -4223,16 +4238,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -4374,16 +4389,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -4525,16 +4540,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -4676,16 +4691,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -4827,16 +4842,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -4975,17 +4990,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4996,8 +5011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5295,7 +5310,7 @@
       </c>
       <c r="G3" s="3">
         <f>'Week (3)'!$H$19</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H3" s="3">
         <f>'Week (4)'!$H$19</f>
@@ -5319,7 +5334,7 @@
       </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3:M5" si="0">SUM(E3:L3)</f>
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5555,7 +5570,7 @@
       </c>
       <c r="G9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H9" s="15">
         <f t="shared" si="3"/>
@@ -5592,7 +5607,7 @@
       <c r="G10" s="20"/>
       <c r="H10" s="20">
         <f>SUM(G2:H8)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20">
@@ -5621,27 +5636,27 @@
       </c>
       <c r="G11" s="18">
         <f t="shared" ref="G11:L11" si="4">F11-G9</f>
-        <v>577.35</v>
+        <v>566.35</v>
       </c>
       <c r="H11" s="18">
         <f t="shared" si="4"/>
-        <v>577.35</v>
+        <v>566.35</v>
       </c>
       <c r="I11" s="18">
         <f t="shared" si="4"/>
-        <v>577.35</v>
+        <v>566.35</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="4"/>
-        <v>577.35</v>
+        <v>566.35</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="4"/>
-        <v>577.35</v>
+        <v>566.35</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="4"/>
-        <v>577.35</v>
+        <v>566.35</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5980,30 +5995,30 @@
         <f>Total!$E$1</f>
         <v>Week 1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -6175,16 +6190,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B13" s="47" t="str">
+      <c r="B13" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
@@ -6337,16 +6352,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B23" s="47" t="str">
+      <c r="B23" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="47"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
@@ -6498,16 +6513,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B32" s="47" t="str">
+      <c r="B32" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="49"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="47"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="str">
@@ -6655,16 +6670,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B41" s="47" t="str">
+      <c r="B41" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="49"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="47"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="str">
@@ -6806,16 +6821,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B50" s="47" t="str">
+      <c r="B50" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="49"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="47"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="str">
@@ -6957,16 +6972,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B59" s="47" t="str">
+      <c r="B59" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="49"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="47"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="str">
@@ -7108,16 +7123,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B68" s="47" t="str">
+      <c r="B68" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="49"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="47"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="str">
@@ -7259,16 +7274,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B77" s="47" t="str">
+      <c r="B77" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C77" s="48"/>
-      <c r="D77" s="48"/>
-      <c r="E77" s="48"/>
-      <c r="F77" s="48"/>
-      <c r="G77" s="48"/>
-      <c r="H77" s="49"/>
+      <c r="C77" s="46"/>
+      <c r="D77" s="46"/>
+      <c r="E77" s="46"/>
+      <c r="F77" s="46"/>
+      <c r="G77" s="46"/>
+      <c r="H77" s="47"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="str">
@@ -7410,16 +7425,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B86" s="47" t="str">
+      <c r="B86" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C86" s="48"/>
-      <c r="D86" s="48"/>
-      <c r="E86" s="48"/>
-      <c r="F86" s="48"/>
-      <c r="G86" s="48"/>
-      <c r="H86" s="49"/>
+      <c r="C86" s="46"/>
+      <c r="D86" s="46"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="46"/>
+      <c r="G86" s="46"/>
+      <c r="H86" s="47"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="str">
@@ -7558,17 +7573,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="B86:H86"/>
     <mergeCell ref="B41:H41"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B59:H59"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7584,7 +7599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D87015-03D4-47DA-AAF3-2136245A2812}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -7853,32 +7868,32 @@
         <f>Total!$F$1</f>
         <v>Week 2</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -8048,16 +8063,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -8216,16 +8231,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -8381,16 +8396,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -8549,16 +8564,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -8702,16 +8717,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -8871,16 +8886,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -9044,16 +9059,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -9195,16 +9210,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -9346,16 +9361,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -9494,17 +9509,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9515,8 +9530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95CCB1C-9FB8-4566-AB28-8B8BAEC7F6E6}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:XFD127"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -9784,32 +9799,32 @@
         <f>Total!$G$1</f>
         <v>Week 3</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -9959,16 +9974,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -10005,47 +10020,63 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="6">
         <f>SUM(B14:G14)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10">
+        <v>2</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="6">
         <f t="shared" ref="H15:H18" si="2">SUM(B15:G15)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10">
+        <v>1.5</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1.5</v>
+      </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -10053,20 +10084,28 @@
       <c r="G17" s="10"/>
       <c r="H17" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="9" t="s">
+        <v>83</v>
+      </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
       <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="10">
+        <v>1.5</v>
+      </c>
       <c r="H18" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -10076,19 +10115,19 @@
       </c>
       <c r="B19" s="11">
         <f t="shared" ref="B19:G19" si="3">SUM(B14:B18)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C19" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D19" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E19" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="3"/>
@@ -10096,11 +10135,11 @@
       </c>
       <c r="G19" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H19" s="11">
         <f>SUM(B19:G19)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
@@ -10108,16 +10147,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -10257,16 +10296,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -10406,16 +10445,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -10557,16 +10596,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -10708,16 +10747,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -10859,16 +10898,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -11010,16 +11049,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -11161,16 +11200,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -11309,17 +11348,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11599,32 +11638,32 @@
         <f>Total!$H$1</f>
         <v>Week 4</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -11774,16 +11813,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -11923,16 +11962,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -12072,16 +12111,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -12221,16 +12260,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -12372,16 +12411,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -12523,16 +12562,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -12674,16 +12713,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -12825,16 +12864,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -12976,16 +13015,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -13124,17 +13163,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13414,31 +13453,31 @@
         <f>Total!$I$1</f>
         <v>Week 5</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -13588,16 +13627,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -13737,16 +13776,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -13886,16 +13925,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -14035,16 +14074,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -14186,16 +14225,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -14337,16 +14376,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -14488,16 +14527,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -14639,16 +14678,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -14790,16 +14829,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -14938,17 +14977,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15228,32 +15267,32 @@
         <f>Total!$J$1</f>
         <v>Week 6</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -15403,16 +15442,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -15552,16 +15591,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -15701,16 +15740,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -15850,16 +15889,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -15998,16 +16037,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -16149,16 +16188,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -16300,16 +16339,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -16451,16 +16490,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -16602,16 +16641,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -16750,17 +16789,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17040,32 +17079,32 @@
         <f>Total!$K$1</f>
         <v>Week 7</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
@@ -17215,16 +17254,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
@@ -17364,16 +17403,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
@@ -17513,16 +17552,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
@@ -17662,16 +17701,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
@@ -17813,16 +17852,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
@@ -17964,16 +18003,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
@@ -18115,16 +18154,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
@@ -18266,16 +18305,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
@@ -18417,16 +18456,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="str">
@@ -18565,17 +18604,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18583,6 +18622,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c6664f9864b54a78bdf9e6230de1c78b>
+    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100294690D6A57C3C4B8650464765815F1C" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="bf1d2ff51e740e451b46e7c13bf9e6da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45f6ce90-ba85-4ef2-b43f-c64448cd95eb" xmlns:ns3="c7549584-aa9c-449c-abfe-2ca02f3a7188" xmlns:ns4="6c73e52c-07d4-4617-ab67-464747257e8d" xmlns:ns5="ab37b2fe-4f81-426e-b942-40459dbac68c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8575fd65d7959dd12bd4dc11d36e634e" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="45f6ce90-ba85-4ef2-b43f-c64448cd95eb"/>
@@ -18825,27 +18884,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c6664f9864b54a78bdf9e6230de1c78b>
-    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
+    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{724CCB8E-5E6A-4B8C-A558-5D9223ADF390}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18864,23 +18922,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
-    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added time register for sprint 1
</commit_message>
<xml_diff>
--- a/2.2_P.CoB_Time_registration_for10.xlsx
+++ b/2.2_P.CoB_Time_registration_for10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\2.2\Client on Board\51\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alira\Desktop\project client on board\Regression-test-management-system\51\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A24FB0-5C87-4C5E-AAC8-4BB1704BE071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B71AE76-D6F5-4E25-8665-B40AF127E95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" tabRatio="835" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="4560" windowWidth="21600" windowHeight="11295" tabRatio="835" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructie" sheetId="19" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>Manual</t>
   </si>
@@ -318,6 +318,27 @@
   </si>
   <si>
     <t>Test case page</t>
+  </si>
+  <si>
+    <t>Added Button comonent</t>
+  </si>
+  <si>
+    <t>client meeting</t>
+  </si>
+  <si>
+    <t>Login page and token and user store,US #8</t>
+  </si>
+  <si>
+    <t>Dashboard Page-front end , US#6</t>
+  </si>
+  <si>
+    <t>Edit sprint page, US #3</t>
+  </si>
+  <si>
+    <t>Sprints page, US #3</t>
+  </si>
+  <si>
+    <t>Refactor the front-end and switch to JS instead of TS</t>
   </si>
 </sst>
 </file>
@@ -823,12 +844,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -837,6 +852,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,10 +984,10 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1919,22 +1940,22 @@
                   <c:v>577.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>545.85</c:v>
+                  <c:v>533.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>545.85</c:v>
+                  <c:v>517.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>545.85</c:v>
+                  <c:v>517.85</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>545.85</c:v>
+                  <c:v>517.85</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>545.85</c:v>
+                  <c:v>517.85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>545.85</c:v>
+                  <c:v>517.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3483,32 +3504,32 @@
         <f>Total!$L$1</f>
         <v>Week 8</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -3658,16 +3679,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -3807,16 +3828,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -3956,16 +3977,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -4105,16 +4126,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -4256,16 +4277,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -4407,16 +4428,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -4558,16 +4579,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -4709,16 +4730,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -4860,16 +4881,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -5008,17 +5029,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5287,11 +5308,11 @@
       </c>
       <c r="G2" s="3">
         <f>'Week (3)'!$H$10</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="H2" s="3">
-        <f>'Week (4)'!$H$10</f>
-        <v>0</v>
+        <f>'Week (4)'!$H$11</f>
+        <v>15.5</v>
       </c>
       <c r="I2" s="3">
         <f>'Week (5)'!$H$10</f>
@@ -5311,7 +5332,7 @@
       </c>
       <c r="M2" s="4">
         <f>SUM(E2:L2)</f>
-        <v>24.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5331,7 +5352,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="3">
-        <f>'Week (4)'!$H$19</f>
+        <f>'Week (4)'!$H$20</f>
         <v>0</v>
       </c>
       <c r="I3" s="3">
@@ -5376,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="3">
-        <f>'Week (4)'!$H$28</f>
+        <f>'Week (4)'!$H$29</f>
         <v>0</v>
       </c>
       <c r="I4" s="3">
@@ -5419,7 +5440,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <f>'Week (4)'!$H$37</f>
+        <f>'Week (4)'!$H$38</f>
         <v>0</v>
       </c>
       <c r="I5" s="3">
@@ -5462,7 +5483,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3">
-        <f>'Week (4)'!$H$46</f>
+        <f>'Week (4)'!$H$47</f>
         <v>0</v>
       </c>
       <c r="I6" s="3">
@@ -5505,7 +5526,7 @@
         <v>8.5</v>
       </c>
       <c r="H7" s="3">
-        <f>'Week (4)'!$H$55</f>
+        <f>'Week (4)'!$H$56</f>
         <v>0</v>
       </c>
       <c r="I7" s="3">
@@ -5548,7 +5569,7 @@
         <v>12</v>
       </c>
       <c r="H8" s="3">
-        <f>'Week (4)'!$H$64</f>
+        <f>'Week (4)'!$H$65</f>
         <v>0</v>
       </c>
       <c r="I8" s="3">
@@ -5588,11 +5609,11 @@
       </c>
       <c r="G9" s="15">
         <f t="shared" si="3"/>
-        <v>31.5</v>
+        <v>44</v>
       </c>
       <c r="H9" s="15">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="3"/>
@@ -5625,7 +5646,7 @@
       <c r="G10" s="20"/>
       <c r="H10" s="20">
         <f>SUM(G2:H8)</f>
-        <v>31.5</v>
+        <v>59.5</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20">
@@ -5654,27 +5675,27 @@
       </c>
       <c r="G11" s="18">
         <f t="shared" ref="G11:L11" si="4">F11-G9</f>
-        <v>545.85</v>
+        <v>533.35</v>
       </c>
       <c r="H11" s="18">
         <f t="shared" si="4"/>
-        <v>545.85</v>
+        <v>517.85</v>
       </c>
       <c r="I11" s="18">
         <f t="shared" si="4"/>
-        <v>545.85</v>
+        <v>517.85</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="4"/>
-        <v>545.85</v>
+        <v>517.85</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="4"/>
-        <v>545.85</v>
+        <v>517.85</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="4"/>
-        <v>545.85</v>
+        <v>517.85</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6013,30 +6034,30 @@
         <f>Total!$E$1</f>
         <v>Week 1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -6208,16 +6229,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B13" s="47" t="str">
+      <c r="B13" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="str">
@@ -6370,16 +6391,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B23" s="47" t="str">
+      <c r="B23" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="47"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="str">
@@ -6531,16 +6552,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B32" s="47" t="str">
+      <c r="B32" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="49"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="47"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
@@ -6688,16 +6709,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B41" s="47" t="str">
+      <c r="B41" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="49"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="47"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="str">
@@ -6839,16 +6860,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B50" s="47" t="str">
+      <c r="B50" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="49"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="47"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="str">
@@ -6990,16 +7011,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B59" s="47" t="str">
+      <c r="B59" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="49"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="47"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="str">
@@ -7141,16 +7162,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B68" s="47" t="str">
+      <c r="B68" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="49"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="47"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="str">
@@ -7292,16 +7313,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B77" s="47" t="str">
+      <c r="B77" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C77" s="48"/>
-      <c r="D77" s="48"/>
-      <c r="E77" s="48"/>
-      <c r="F77" s="48"/>
-      <c r="G77" s="48"/>
-      <c r="H77" s="49"/>
+      <c r="C77" s="46"/>
+      <c r="D77" s="46"/>
+      <c r="E77" s="46"/>
+      <c r="F77" s="46"/>
+      <c r="G77" s="46"/>
+      <c r="H77" s="47"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="str">
@@ -7443,16 +7464,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B86" s="47" t="str">
+      <c r="B86" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C86" s="48"/>
-      <c r="D86" s="48"/>
-      <c r="E86" s="48"/>
-      <c r="F86" s="48"/>
-      <c r="G86" s="48"/>
-      <c r="H86" s="49"/>
+      <c r="C86" s="46"/>
+      <c r="D86" s="46"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="46"/>
+      <c r="G86" s="46"/>
+      <c r="H86" s="47"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="str">
@@ -7591,17 +7612,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="B86:H86"/>
     <mergeCell ref="B41:H41"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B59:H59"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7617,7 +7638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D87015-03D4-47DA-AAF3-2136245A2812}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A50" sqref="A50:G54"/>
     </sheetView>
   </sheetViews>
@@ -7886,32 +7907,32 @@
         <f>Total!$F$1</f>
         <v>Week 2</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -8081,16 +8102,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -8252,16 +8273,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -8417,16 +8438,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -8585,16 +8606,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -8738,16 +8759,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -8907,16 +8928,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -9080,16 +9101,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -9231,16 +9252,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -9382,16 +9403,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -9530,17 +9551,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9551,8 +9572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95CCB1C-9FB8-4566-AB28-8B8BAEC7F6E6}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -9820,32 +9841,32 @@
         <f>Total!$G$1</f>
         <v>Week 3</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -9882,8 +9903,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -9891,59 +9916,76 @@
       <c r="G5" s="10"/>
       <c r="H5" s="6">
         <f>SUM(B5:G5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
       <c r="H6" s="6">
         <f t="shared" ref="H6:H9" si="0">SUM(B6:G6)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10">
+        <v>2</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -9953,31 +9995,31 @@
       </c>
       <c r="B10" s="11">
         <f t="shared" ref="B10:G10" si="1">SUM(B5:B9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H10" s="11">
         <f>SUM(B10:G10)</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -9995,16 +10037,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -10168,16 +10210,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -10317,16 +10359,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -10466,16 +10508,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -10617,16 +10659,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -10778,16 +10820,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -10941,16 +10983,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -11092,16 +11134,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -11243,16 +11285,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -11391,17 +11433,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11410,10 +11452,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB66144-3102-4D48-A4D0-FA37996B20EF}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:XFD129"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11681,32 +11723,32 @@
         <f>Total!$H$1</f>
         <v>Week 4</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -11743,47 +11785,62 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10">
+        <v>4</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="6">
         <f>SUM(B5:G5)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="6">
-        <f t="shared" ref="H6:H9" si="0">SUM(B6:G6)</f>
-        <v>0</v>
+        <f t="shared" ref="H6:H10" si="0">SUM(B6:G6)</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10">
+        <v>2</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="10">
+        <v>4</v>
+      </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -11791,127 +11848,132 @@
       <c r="G8" s="10"/>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
       <c r="G9" s="10"/>
-      <c r="H9" s="6">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="str">
         <f>'Week (1)'!$A$11</f>
         <v>Total</v>
       </c>
-      <c r="B10" s="11">
-        <f t="shared" ref="B10:G10" si="1">SUM(B5:B9)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
-        <f>SUM(B10:G10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="str">
+      <c r="B11" s="11">
+        <f>SUM(B5:B10)</f>
+        <v>4</v>
+      </c>
+      <c r="C11" s="11">
+        <f>SUM(C5:C10)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="11">
+        <f>SUM(D5:D10)</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="11">
+        <f>SUM(E5:E10)</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="11">
+        <f>SUM(F5:F10)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="11">
+        <f>SUM(G5:G10)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="11">
+        <f>SUM(B11:G11)</f>
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="str">
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B13" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="str">
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="str">
         <f>'Week (1)'!$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B13" s="8" t="str">
+      <c r="B14" s="8" t="str">
         <f>'Week (1)'!B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C13" s="8" t="str">
+      <c r="C14" s="8" t="str">
         <f>'Week (1)'!C$4</f>
         <v>Di</v>
       </c>
-      <c r="D13" s="8" t="str">
+      <c r="D14" s="8" t="str">
         <f>'Week (1)'!D$4</f>
         <v>Wo</v>
       </c>
-      <c r="E13" s="8" t="str">
+      <c r="E14" s="8" t="str">
         <f>'Week (1)'!E$4</f>
         <v>Do</v>
       </c>
-      <c r="F13" s="8" t="str">
+      <c r="F14" s="8" t="str">
         <f>'Week (1)'!F$4</f>
         <v>Vr</v>
       </c>
-      <c r="G13" s="8" t="str">
+      <c r="G14" s="8" t="str">
         <f>'Week (1)'!G$4</f>
         <v>Za/Zo</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="H14" s="8" t="str">
         <f>'Week (1)'!H$4</f>
         <v>Total</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="6">
-        <f>SUM(B14:G14)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -11923,7 +11985,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="6">
-        <f t="shared" ref="H15:H18" si="2">SUM(B15:G15)</f>
+        <f>SUM(B15:G15)</f>
         <v>0</v>
       </c>
     </row>
@@ -11936,7 +11998,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H16:H19" si="1">SUM(B16:G16)</f>
         <v>0</v>
       </c>
     </row>
@@ -11949,7 +12011,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -11962,105 +12024,105 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="str">
         <f>'Week (1)'!$A$11</f>
         <v>Total</v>
       </c>
-      <c r="B19" s="11">
-        <f t="shared" ref="B19:G19" si="3">SUM(B14:B18)</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="11">
-        <f>SUM(B19:G19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="str">
+      <c r="B20" s="11">
+        <f t="shared" ref="B20:G20" si="2">SUM(B15:B19)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <f>SUM(B20:G20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="str">
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B22" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="str">
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="str">
         <f>'Week (1)'!$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B22" s="8" t="str">
+      <c r="B23" s="8" t="str">
         <f>'Week (1)'!B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C22" s="8" t="str">
+      <c r="C23" s="8" t="str">
         <f>'Week (1)'!C$4</f>
         <v>Di</v>
       </c>
-      <c r="D22" s="8" t="str">
+      <c r="D23" s="8" t="str">
         <f>'Week (1)'!D$4</f>
         <v>Wo</v>
       </c>
-      <c r="E22" s="8" t="str">
+      <c r="E23" s="8" t="str">
         <f>'Week (1)'!E$4</f>
         <v>Do</v>
       </c>
-      <c r="F22" s="8" t="str">
+      <c r="F23" s="8" t="str">
         <f>'Week (1)'!F$4</f>
         <v>Vr</v>
       </c>
-      <c r="G22" s="8" t="str">
+      <c r="G23" s="8" t="str">
         <f>'Week (1)'!G$4</f>
         <v>Za/Zo</v>
       </c>
-      <c r="H22" s="8" t="str">
+      <c r="H23" s="8" t="str">
         <f>'Week (1)'!H$4</f>
         <v>Total</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="6">
-        <f>SUM(B23:G23)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -12072,7 +12134,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="6">
-        <f t="shared" ref="H24:H27" si="4">SUM(B24:G24)</f>
+        <f>SUM(B24:G24)</f>
         <v>0</v>
       </c>
     </row>
@@ -12085,7 +12147,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H25:H28" si="3">SUM(B25:G25)</f>
         <v>0</v>
       </c>
     </row>
@@ -12098,7 +12160,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12111,105 +12173,105 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="str">
         <f>'Week (1)'!$A$11</f>
         <v>Total</v>
       </c>
-      <c r="B28" s="11">
-        <f t="shared" ref="B28:G28" si="5">SUM(B23:B27)</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D28" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
-        <f>SUM(B28:G28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="str">
+      <c r="B29" s="11">
+        <f t="shared" ref="B29:G29" si="4">SUM(B24:B28)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="11">
+        <f>SUM(B29:G29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="str">
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B31" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="str">
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="str">
         <f>'Week (1)'!$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B31" s="8" t="str">
+      <c r="B32" s="8" t="str">
         <f>'Week (1)'!B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C31" s="8" t="str">
+      <c r="C32" s="8" t="str">
         <f>'Week (1)'!C$4</f>
         <v>Di</v>
       </c>
-      <c r="D31" s="8" t="str">
+      <c r="D32" s="8" t="str">
         <f>'Week (1)'!D$4</f>
         <v>Wo</v>
       </c>
-      <c r="E31" s="8" t="str">
+      <c r="E32" s="8" t="str">
         <f>'Week (1)'!E$4</f>
         <v>Do</v>
       </c>
-      <c r="F31" s="8" t="str">
+      <c r="F32" s="8" t="str">
         <f>'Week (1)'!F$4</f>
         <v>Vr</v>
       </c>
-      <c r="G31" s="8" t="str">
+      <c r="G32" s="8" t="str">
         <f>'Week (1)'!G$4</f>
         <v>Za/Zo</v>
       </c>
-      <c r="H31" s="8" t="str">
+      <c r="H32" s="8" t="str">
         <f>'Week (1)'!H$4</f>
         <v>Total</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="6">
-        <f>SUM(B32:G32)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -12221,7 +12283,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="6">
-        <f t="shared" ref="H33:H36" si="6">SUM(B33:G33)</f>
+        <f>SUM(B33:G33)</f>
         <v>0</v>
       </c>
     </row>
@@ -12234,7 +12296,7 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H34:H37" si="5">SUM(B34:G34)</f>
         <v>0</v>
       </c>
     </row>
@@ -12247,7 +12309,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -12260,111 +12322,111 @@
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="str">
         <f>'Week (1)'!$A$11</f>
         <v>Total</v>
       </c>
-      <c r="B37" s="11">
-        <f t="shared" ref="B37:G37" si="7">SUM(B32:B36)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="11">
-        <f>SUM(B37:G37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="str">
+      <c r="B38" s="11">
+        <f t="shared" ref="B38:G38" si="6">SUM(B33:B37)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="11">
+        <f>SUM(B38:G38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="str">
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B40" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="str">
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="47"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="str">
         <f>$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B40" s="8" t="str">
+      <c r="B41" s="8" t="str">
         <f>B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C40" s="8" t="str">
-        <f t="shared" ref="C40:H40" si="8">C$4</f>
+      <c r="C41" s="8" t="str">
+        <f t="shared" ref="C41:H41" si="7">C$4</f>
         <v>Di</v>
       </c>
-      <c r="D40" s="8" t="str">
-        <f t="shared" si="8"/>
+      <c r="D41" s="8" t="str">
+        <f t="shared" si="7"/>
         <v>Wo</v>
       </c>
-      <c r="E40" s="8" t="str">
-        <f t="shared" si="8"/>
+      <c r="E41" s="8" t="str">
+        <f t="shared" si="7"/>
         <v>Do</v>
       </c>
-      <c r="F40" s="8" t="str">
-        <f t="shared" si="8"/>
+      <c r="F41" s="8" t="str">
+        <f t="shared" si="7"/>
         <v>Vr</v>
       </c>
-      <c r="G40" s="8" t="str">
-        <f t="shared" si="8"/>
+      <c r="G41" s="8" t="str">
+        <f t="shared" si="7"/>
         <v>Za/Zo</v>
       </c>
-      <c r="H40" s="8" t="str">
-        <f t="shared" si="8"/>
+      <c r="H41" s="8" t="str">
+        <f t="shared" si="7"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="6">
-        <f>SUM(B41:G41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -12372,7 +12434,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="6">
-        <f t="shared" ref="H42:H45" si="9">SUM(B42:G42)</f>
+        <f>SUM(B42:G42)</f>
         <v>0</v>
       </c>
     </row>
@@ -12385,7 +12447,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="H43:H46" si="8">SUM(B43:G43)</f>
         <v>0</v>
       </c>
     </row>
@@ -12398,7 +12460,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -12411,111 +12473,111 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="str">
+        <f>$A$11</f>
+        <v>Total</v>
+      </c>
+      <c r="B47" s="11">
+        <f t="shared" ref="B47:G47" si="9">SUM(B42:B46)</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="str">
-        <f>$A$10</f>
-        <v>Total</v>
-      </c>
-      <c r="B46" s="11">
-        <f t="shared" ref="B46:G46" si="10">SUM(B41:B45)</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="D46" s="11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H46" s="11">
-        <f>SUM(B46:G46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="12" t="str">
+      <c r="D47" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H47" s="11">
+        <f>SUM(B47:G47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="str">
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B49" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="str">
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="47"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="str">
         <f>$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B49" s="8" t="str">
+      <c r="B50" s="8" t="str">
         <f>B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C49" s="8" t="str">
-        <f t="shared" ref="C49:H49" si="11">C$4</f>
+      <c r="C50" s="8" t="str">
+        <f t="shared" ref="C50:H50" si="10">C$4</f>
         <v>Di</v>
       </c>
-      <c r="D49" s="8" t="str">
-        <f t="shared" si="11"/>
+      <c r="D50" s="8" t="str">
+        <f t="shared" si="10"/>
         <v>Wo</v>
       </c>
-      <c r="E49" s="8" t="str">
-        <f t="shared" si="11"/>
+      <c r="E50" s="8" t="str">
+        <f t="shared" si="10"/>
         <v>Do</v>
       </c>
-      <c r="F49" s="8" t="str">
-        <f t="shared" si="11"/>
+      <c r="F50" s="8" t="str">
+        <f t="shared" si="10"/>
         <v>Vr</v>
       </c>
-      <c r="G49" s="8" t="str">
-        <f t="shared" si="11"/>
+      <c r="G50" s="8" t="str">
+        <f t="shared" si="10"/>
         <v>Za/Zo</v>
       </c>
-      <c r="H49" s="8" t="str">
-        <f t="shared" si="11"/>
+      <c r="H50" s="8" t="str">
+        <f t="shared" si="10"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="6">
-        <f>SUM(B50:G50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -12523,7 +12585,7 @@
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="6">
-        <f t="shared" ref="H51:H54" si="12">SUM(B51:G51)</f>
+        <f>SUM(B51:G51)</f>
         <v>0</v>
       </c>
     </row>
@@ -12536,7 +12598,7 @@
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="H52:H55" si="11">SUM(B52:G52)</f>
         <v>0</v>
       </c>
     </row>
@@ -12549,7 +12611,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
       <c r="H53" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -12562,111 +12624,111 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="21" t="str">
+        <f>$A$11</f>
+        <v>Total</v>
+      </c>
+      <c r="B56" s="11">
+        <f t="shared" ref="B56:G56" si="12">SUM(B51:B55)</f>
+        <v>0</v>
+      </c>
+      <c r="C56" s="11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="21" t="str">
-        <f>$A$10</f>
-        <v>Total</v>
-      </c>
-      <c r="B55" s="11">
-        <f t="shared" ref="B55:G55" si="13">SUM(B50:B54)</f>
-        <v>0</v>
-      </c>
-      <c r="C55" s="11">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="D55" s="11">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="11">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="F55" s="11">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="G55" s="11">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="H55" s="11">
-        <f>SUM(B55:G55)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="12" t="str">
+      <c r="D56" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E56" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H56" s="11">
+        <f>SUM(B56:G56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="12" t="str">
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B58" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="str">
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="47"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="str">
         <f>$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B58" s="8" t="str">
+      <c r="B59" s="8" t="str">
         <f>B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C58" s="8" t="str">
-        <f t="shared" ref="C58:H58" si="14">C$4</f>
+      <c r="C59" s="8" t="str">
+        <f t="shared" ref="C59:H59" si="13">C$4</f>
         <v>Di</v>
       </c>
-      <c r="D58" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="D59" s="8" t="str">
+        <f t="shared" si="13"/>
         <v>Wo</v>
       </c>
-      <c r="E58" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="E59" s="8" t="str">
+        <f t="shared" si="13"/>
         <v>Do</v>
       </c>
-      <c r="F58" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="F59" s="8" t="str">
+        <f t="shared" si="13"/>
         <v>Vr</v>
       </c>
-      <c r="G58" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="G59" s="8" t="str">
+        <f t="shared" si="13"/>
         <v>Za/Zo</v>
       </c>
-      <c r="H58" s="8" t="str">
-        <f t="shared" si="14"/>
+      <c r="H59" s="8" t="str">
+        <f t="shared" si="13"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="6">
-        <f>SUM(B59:G59)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -12674,7 +12736,7 @@
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="6">
-        <f t="shared" ref="H60:H63" si="15">SUM(B60:G60)</f>
+        <f>SUM(B60:G60)</f>
         <v>0</v>
       </c>
     </row>
@@ -12687,7 +12749,7 @@
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="H61:H64" si="14">SUM(B61:G61)</f>
         <v>0</v>
       </c>
     </row>
@@ -12700,7 +12762,7 @@
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
       <c r="H62" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -12713,111 +12775,111 @@
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="9"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="6">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="21" t="str">
+        <f>$A$11</f>
+        <v>Total</v>
+      </c>
+      <c r="B65" s="11">
+        <f t="shared" ref="B65:G65" si="15">SUM(B60:B64)</f>
+        <v>0</v>
+      </c>
+      <c r="C65" s="11">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="21" t="str">
-        <f>$A$10</f>
-        <v>Total</v>
-      </c>
-      <c r="B64" s="11">
-        <f t="shared" ref="B64:G64" si="16">SUM(B59:B63)</f>
-        <v>0</v>
-      </c>
-      <c r="C64" s="11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="D64" s="11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="E64" s="11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="F64" s="11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="G64" s="11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H64" s="11">
-        <f>SUM(B64:G64)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A66" s="12" t="e">
+      <c r="D65" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E65" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="11">
+        <f>SUM(B65:G65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A67" s="12" t="e">
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B67" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="str">
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="47"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="str">
         <f>$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B67" s="8" t="str">
+      <c r="B68" s="8" t="str">
         <f>B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C67" s="8" t="str">
-        <f t="shared" ref="C67:H67" si="17">C$4</f>
+      <c r="C68" s="8" t="str">
+        <f t="shared" ref="C68:H68" si="16">C$4</f>
         <v>Di</v>
       </c>
-      <c r="D67" s="8" t="str">
-        <f t="shared" si="17"/>
+      <c r="D68" s="8" t="str">
+        <f t="shared" si="16"/>
         <v>Wo</v>
       </c>
-      <c r="E67" s="8" t="str">
-        <f t="shared" si="17"/>
+      <c r="E68" s="8" t="str">
+        <f t="shared" si="16"/>
         <v>Do</v>
       </c>
-      <c r="F67" s="8" t="str">
-        <f t="shared" si="17"/>
+      <c r="F68" s="8" t="str">
+        <f t="shared" si="16"/>
         <v>Vr</v>
       </c>
-      <c r="G67" s="8" t="str">
-        <f t="shared" si="17"/>
+      <c r="G68" s="8" t="str">
+        <f t="shared" si="16"/>
         <v>Za/Zo</v>
       </c>
-      <c r="H67" s="8" t="str">
-        <f t="shared" si="17"/>
+      <c r="H68" s="8" t="str">
+        <f t="shared" si="16"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
-      <c r="H68" s="6">
-        <f>SUM(B68:G68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="9"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -12825,7 +12887,7 @@
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
       <c r="H69" s="6">
-        <f t="shared" ref="H69:H72" si="18">SUM(B69:G69)</f>
+        <f>SUM(B69:G69)</f>
         <v>0</v>
       </c>
     </row>
@@ -12838,7 +12900,7 @@
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
       <c r="H70" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="H70:H73" si="17">SUM(B70:G70)</f>
         <v>0</v>
       </c>
     </row>
@@ -12851,7 +12913,7 @@
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
       <c r="H71" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -12864,111 +12926,111 @@
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
       <c r="H72" s="6">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="9"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="6">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="21" t="str">
+        <f>$A$11</f>
+        <v>Total</v>
+      </c>
+      <c r="B74" s="11">
+        <f t="shared" ref="B74:G74" si="18">SUM(B69:B73)</f>
+        <v>0</v>
+      </c>
+      <c r="C74" s="11">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="21" t="str">
-        <f>$A$10</f>
-        <v>Total</v>
-      </c>
-      <c r="B73" s="11">
-        <f t="shared" ref="B73:G73" si="19">SUM(B68:B72)</f>
-        <v>0</v>
-      </c>
-      <c r="C73" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="D73" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="E73" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="F73" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="G73" s="11">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="H73" s="11">
-        <f>SUM(B73:G73)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A75" s="12" t="e">
+      <c r="D74" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E74" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="F74" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G74" s="11">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H74" s="11">
+        <f>SUM(B74:G74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A76" s="12" t="e">
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B76" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="str">
+      <c r="C76" s="46"/>
+      <c r="D76" s="46"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="46"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="47"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="str">
         <f>$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B76" s="8" t="str">
+      <c r="B77" s="8" t="str">
         <f>B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C76" s="8" t="str">
-        <f t="shared" ref="C76:H76" si="20">C$4</f>
+      <c r="C77" s="8" t="str">
+        <f t="shared" ref="C77:H77" si="19">C$4</f>
         <v>Di</v>
       </c>
-      <c r="D76" s="8" t="str">
-        <f t="shared" si="20"/>
+      <c r="D77" s="8" t="str">
+        <f t="shared" si="19"/>
         <v>Wo</v>
       </c>
-      <c r="E76" s="8" t="str">
-        <f t="shared" si="20"/>
+      <c r="E77" s="8" t="str">
+        <f t="shared" si="19"/>
         <v>Do</v>
       </c>
-      <c r="F76" s="8" t="str">
-        <f t="shared" si="20"/>
+      <c r="F77" s="8" t="str">
+        <f t="shared" si="19"/>
         <v>Vr</v>
       </c>
-      <c r="G76" s="8" t="str">
-        <f t="shared" si="20"/>
+      <c r="G77" s="8" t="str">
+        <f t="shared" si="19"/>
         <v>Za/Zo</v>
       </c>
-      <c r="H76" s="8" t="str">
-        <f t="shared" si="20"/>
+      <c r="H77" s="8" t="str">
+        <f t="shared" si="19"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="6">
-        <f>SUM(B77:G77)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
@@ -12976,7 +13038,7 @@
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
       <c r="H78" s="6">
-        <f t="shared" ref="H78:H81" si="21">SUM(B78:G78)</f>
+        <f>SUM(B78:G78)</f>
         <v>0</v>
       </c>
     </row>
@@ -12989,7 +13051,7 @@
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
       <c r="H79" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="H79:H82" si="20">SUM(B79:G79)</f>
         <v>0</v>
       </c>
     </row>
@@ -13002,7 +13064,7 @@
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
       <c r="H80" s="6">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -13015,111 +13077,111 @@
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
       <c r="H81" s="6">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="9"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="6">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="21" t="str">
+        <f>$A$11</f>
+        <v>Total</v>
+      </c>
+      <c r="B83" s="11">
+        <f t="shared" ref="B83:G83" si="21">SUM(B78:B82)</f>
+        <v>0</v>
+      </c>
+      <c r="C83" s="11">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="21" t="str">
-        <f>$A$10</f>
-        <v>Total</v>
-      </c>
-      <c r="B82" s="11">
-        <f t="shared" ref="B82:G82" si="22">SUM(B77:B81)</f>
-        <v>0</v>
-      </c>
-      <c r="C82" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="D82" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="E82" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="F82" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="G82" s="11">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="H82" s="11">
-        <f>SUM(B82:G82)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A84" s="12" t="e">
+      <c r="D83" s="11">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="11">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="11">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G83" s="11">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H83" s="11">
+        <f>SUM(B83:G83)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A85" s="12" t="e">
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B85" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="str">
+      <c r="C85" s="46"/>
+      <c r="D85" s="46"/>
+      <c r="E85" s="46"/>
+      <c r="F85" s="46"/>
+      <c r="G85" s="46"/>
+      <c r="H85" s="47"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="str">
         <f>$A$4</f>
         <v>User story / task description</v>
       </c>
-      <c r="B85" s="8" t="str">
+      <c r="B86" s="8" t="str">
         <f>B$4</f>
         <v>Ma</v>
       </c>
-      <c r="C85" s="8" t="str">
-        <f t="shared" ref="C85:H85" si="23">C$4</f>
+      <c r="C86" s="8" t="str">
+        <f t="shared" ref="C86:H86" si="22">C$4</f>
         <v>Di</v>
       </c>
-      <c r="D85" s="8" t="str">
-        <f t="shared" si="23"/>
+      <c r="D86" s="8" t="str">
+        <f t="shared" si="22"/>
         <v>Wo</v>
       </c>
-      <c r="E85" s="8" t="str">
-        <f t="shared" si="23"/>
+      <c r="E86" s="8" t="str">
+        <f t="shared" si="22"/>
         <v>Do</v>
       </c>
-      <c r="F85" s="8" t="str">
-        <f t="shared" si="23"/>
+      <c r="F86" s="8" t="str">
+        <f t="shared" si="22"/>
         <v>Vr</v>
       </c>
-      <c r="G85" s="8" t="str">
-        <f t="shared" si="23"/>
+      <c r="G86" s="8" t="str">
+        <f t="shared" si="22"/>
         <v>Za/Zo</v>
       </c>
-      <c r="H85" s="8" t="str">
-        <f t="shared" si="23"/>
+      <c r="H86" s="8" t="str">
+        <f t="shared" si="22"/>
         <v>Total</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="9" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="10"/>
-      <c r="H86" s="6">
-        <f>SUM(B86:G86)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="9"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
@@ -13127,7 +13189,7 @@
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
       <c r="H87" s="6">
-        <f t="shared" ref="H87:H90" si="24">SUM(B87:G87)</f>
+        <f>SUM(B87:G87)</f>
         <v>0</v>
       </c>
     </row>
@@ -13140,7 +13202,7 @@
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
       <c r="H88" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="H88:H91" si="23">SUM(B88:G88)</f>
         <v>0</v>
       </c>
     </row>
@@ -13153,7 +13215,7 @@
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
       <c r="H89" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -13166,57 +13228,70 @@
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
       <c r="H90" s="6">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="9"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="6">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="21" t="str">
+        <f>$A$11</f>
+        <v>Total</v>
+      </c>
+      <c r="B92" s="11">
+        <f t="shared" ref="B92:G92" si="24">SUM(B87:B91)</f>
+        <v>0</v>
+      </c>
+      <c r="C92" s="11">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="21" t="str">
-        <f>$A$10</f>
-        <v>Total</v>
-      </c>
-      <c r="B91" s="11">
-        <f t="shared" ref="B91:G91" si="25">SUM(B86:B90)</f>
-        <v>0</v>
-      </c>
-      <c r="C91" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="D91" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="E91" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="F91" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="11">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="H91" s="11">
-        <f>SUM(B91:G91)</f>
+      <c r="D92" s="11">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="11">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="F92" s="11">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="G92" s="11">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="H92" s="11">
+        <f>SUM(B92:G92)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B48:H48"/>
-    <mergeCell ref="B57:H57"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="B75:H75"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="B76:H76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13496,31 +13571,31 @@
         <f>Total!$I$1</f>
         <v>Week 5</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -13670,16 +13745,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -13819,16 +13894,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -13968,16 +14043,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -14117,16 +14192,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -14268,16 +14343,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -14419,16 +14494,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -14570,16 +14645,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -14721,16 +14796,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -14872,16 +14947,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -15020,17 +15095,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15310,32 +15385,32 @@
         <f>Total!$J$1</f>
         <v>Week 6</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -15485,16 +15560,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -15634,16 +15709,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -15783,16 +15858,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -15932,16 +16007,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -16080,16 +16155,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -16231,16 +16306,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -16382,16 +16457,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -16533,16 +16608,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -16684,16 +16759,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -16832,17 +16907,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17122,32 +17197,32 @@
         <f>Total!$K$1</f>
         <v>Week 7</v>
       </c>
-      <c r="B1" s="45" t="str">
+      <c r="B1" s="48" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -17297,16 +17372,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -17446,16 +17521,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="47" t="str">
+      <c r="B21" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -17595,16 +17670,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="47" t="str">
+      <c r="B30" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -17744,16 +17819,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="47" t="str">
+      <c r="B39" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -17895,16 +17970,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="47" t="str">
+      <c r="B48" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="49"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -18046,16 +18121,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="47" t="str">
+      <c r="B57" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="49"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -18197,16 +18272,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="47" t="str">
+      <c r="B66" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="49"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -18348,16 +18423,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="47" t="str">
+      <c r="B75" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="49"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -18499,16 +18574,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="47" t="str">
+      <c r="B84" s="45" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="49"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -18647,17 +18722,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18665,6 +18740,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c6664f9864b54a78bdf9e6230de1c78b>
+    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100294690D6A57C3C4B8650464765815F1C" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="bf1d2ff51e740e451b46e7c13bf9e6da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45f6ce90-ba85-4ef2-b43f-c64448cd95eb" xmlns:ns3="c7549584-aa9c-449c-abfe-2ca02f3a7188" xmlns:ns4="6c73e52c-07d4-4617-ab67-464747257e8d" xmlns:ns5="ab37b2fe-4f81-426e-b942-40459dbac68c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8575fd65d7959dd12bd4dc11d36e634e" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="45f6ce90-ba85-4ef2-b43f-c64448cd95eb"/>
@@ -18907,27 +19002,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c6664f9864b54a78bdf9e6230de1c78b>
-    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
+    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{724CCB8E-5E6A-4B8C-A558-5D9223ADF390}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18946,23 +19040,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
-    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
time registration + retrospective
</commit_message>
<xml_diff>
--- a/2.2_P.CoB_Time_registration_for10.xlsx
+++ b/2.2_P.CoB_Time_registration_for10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\OneDrive\Documentos\GitHub\Client_Board\51\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ferhat Kelten\Desktop\51\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C82A71-1388-434F-B14F-C87AB6252C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3A5A67-C100-47FE-AD80-FCC713A49921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="835" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37665" windowHeight="21840" tabRatio="835" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructie" sheetId="19" r:id="rId1"/>
@@ -24,10 +24,21 @@
     <sheet name="Week (7)" sheetId="25" r:id="rId9"/>
     <sheet name="Week (8)" sheetId="26" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="169">
   <si>
     <t>Manual</t>
   </si>
@@ -532,6 +543,18 @@
   </si>
   <si>
     <t>1.3</t>
+  </si>
+  <si>
+    <t>Fixing bugs on API calls</t>
+  </si>
+  <si>
+    <t>Working on backend</t>
+  </si>
+  <si>
+    <t>Charts</t>
+  </si>
+  <si>
+    <t>Editing test steps</t>
   </si>
 </sst>
 </file>
@@ -1044,12 +1067,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1058,6 +1075,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1084,7 +1107,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1703,19 +1726,19 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1994,7 +2017,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2060,7 +2083,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2143,19 +2166,19 @@
                   <c:v>479.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>415.05</c:v>
+                  <c:v>405.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>343.05</c:v>
+                  <c:v>328.05</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>247.55</c:v>
+                  <c:v>217.55</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>169.65</c:v>
+                  <c:v>138.65</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>124.95</c:v>
+                  <c:v>83.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2301,7 +2324,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="82118767"/>
@@ -2360,7 +2383,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="82118351"/>
@@ -2402,7 +2425,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2436,7 +2459,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3373,7 +3396,7 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
   </cols>
@@ -3435,11 +3458,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A799882-C011-443F-BBA4-4F4C207196D0}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -3704,32 +3727,32 @@
         <f>Total!$L$1</f>
         <v>Week 8</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -3879,16 +3902,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="48" t="str">
+      <c r="B12" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -4032,16 +4055,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="48" t="str">
+      <c r="B21" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -4181,16 +4204,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="48" t="str">
+      <c r="B30" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="50"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -4360,16 +4383,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="48" t="str">
+      <c r="B39" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="50"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -4511,16 +4534,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="48" t="str">
+      <c r="B48" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -4688,16 +4711,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="48" t="str">
+      <c r="B57" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="50"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="48"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -4735,43 +4758,61 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
+      <c r="C59" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="6">
         <f>SUM(B59:G59)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="9"/>
-      <c r="B60" s="10"/>
+      <c r="A60" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="10">
+        <v>1</v>
+      </c>
       <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
+      <c r="D60" s="10">
+        <v>1</v>
+      </c>
       <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+      <c r="F60" s="10">
+        <v>1</v>
+      </c>
+      <c r="G60" s="10">
+        <v>2</v>
+      </c>
       <c r="H60" s="6">
         <f t="shared" ref="H60:H63" si="15">SUM(B60:G60)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
+      <c r="A61" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
+      <c r="C61" s="10">
+        <v>1</v>
+      </c>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
+      <c r="F61" s="10">
+        <v>2</v>
+      </c>
       <c r="G61" s="10"/>
       <c r="H61" s="6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -4807,15 +4848,15 @@
       </c>
       <c r="B64" s="11">
         <f t="shared" ref="B64:G64" si="16">SUM(B59:B63)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="D64" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="11">
         <f t="shared" si="16"/>
@@ -4823,15 +4864,15 @@
       </c>
       <c r="F64" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G64" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H64" s="11">
         <f>SUM(B64:G64)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
@@ -4839,16 +4880,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="48" t="str">
+      <c r="B66" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="50"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="48"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -4990,16 +5031,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="48" t="str">
+      <c r="B75" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="50"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -5141,16 +5182,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="48" t="str">
+      <c r="B84" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
-      <c r="H84" s="50"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="48"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -5289,17 +5330,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5314,7 +5355,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" style="28" customWidth="1"/>
     <col min="2" max="2" width="65.7109375" customWidth="1"/>
@@ -5830,27 +5871,27 @@
       </c>
       <c r="H8" s="3">
         <f>'Week (4)'!$H$65</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I8" s="3">
         <f>'Week (5)'!$H$63</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J8" s="3">
         <f>'Week (6)'!$H$65</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K8" s="3">
         <f>'Week (7)'!$H$64</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="3">
         <f>'Week (8)'!$H$64</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5873,23 +5914,23 @@
       </c>
       <c r="H9" s="15">
         <f t="shared" si="3"/>
-        <v>64.2</v>
+        <v>74.2</v>
       </c>
       <c r="I9" s="15">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="J9" s="15">
         <f t="shared" si="3"/>
-        <v>95.5</v>
+        <v>110.5</v>
       </c>
       <c r="K9" s="15">
         <f t="shared" si="3"/>
-        <v>77.900000000000006</v>
+        <v>78.900000000000006</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" si="3"/>
-        <v>44.7</v>
+        <v>55.2</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5906,17 +5947,17 @@
       <c r="G10" s="20"/>
       <c r="H10" s="20">
         <f>SUM(G2:H8)</f>
-        <v>133.19999999999999</v>
+        <v>143.19999999999999</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="20">
         <f>SUM(I2:J8)</f>
-        <v>167.5</v>
+        <v>187.5</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="20">
         <f>SUM(K9:L9)</f>
-        <v>122.60000000000001</v>
+        <v>134.10000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5939,23 +5980,23 @@
       </c>
       <c r="H11" s="18">
         <f t="shared" si="4"/>
-        <v>415.05</v>
+        <v>405.05</v>
       </c>
       <c r="I11" s="18">
         <f t="shared" si="4"/>
-        <v>343.05</v>
+        <v>328.05</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="4"/>
-        <v>247.55</v>
+        <v>217.55</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="4"/>
-        <v>169.65</v>
+        <v>138.65</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="4"/>
-        <v>124.95</v>
+        <v>83.45</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6029,7 +6070,7 @@
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -6294,30 +6335,30 @@
         <f>Total!$E$1</f>
         <v>Week 1</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -6489,16 +6530,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B13" s="48" t="str">
+      <c r="B13" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="str">
@@ -6651,16 +6692,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B23" s="48" t="str">
+      <c r="B23" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="50"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="str">
@@ -6812,16 +6853,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B32" s="48" t="str">
+      <c r="B32" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="50"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="48"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
@@ -6973,16 +7014,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B41" s="48" t="str">
+      <c r="B41" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="50"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="48"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="str">
@@ -7144,16 +7185,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B50" s="48" t="str">
+      <c r="B50" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="50"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="48"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="str">
@@ -7309,16 +7350,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B59" s="48" t="str">
+      <c r="B59" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="50"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="48"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="str">
@@ -7460,16 +7501,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B68" s="48" t="str">
+      <c r="B68" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="50"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="48"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="str">
@@ -7611,16 +7652,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B77" s="48" t="str">
+      <c r="B77" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C77" s="49"/>
-      <c r="D77" s="49"/>
-      <c r="E77" s="49"/>
-      <c r="F77" s="49"/>
-      <c r="G77" s="49"/>
-      <c r="H77" s="50"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="47"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="47"/>
+      <c r="H77" s="48"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="str">
@@ -7762,16 +7803,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B86" s="48" t="str">
+      <c r="B86" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C86" s="49"/>
-      <c r="D86" s="49"/>
-      <c r="E86" s="49"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="49"/>
-      <c r="H86" s="50"/>
+      <c r="C86" s="47"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="47"/>
+      <c r="F86" s="47"/>
+      <c r="G86" s="47"/>
+      <c r="H86" s="48"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="str">
@@ -7910,17 +7951,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="B86:H86"/>
     <mergeCell ref="B41:H41"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B59:H59"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7940,7 +7981,7 @@
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -8205,32 +8246,32 @@
         <f>Total!$F$1</f>
         <v>Week 2</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -8400,16 +8441,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="48" t="str">
+      <c r="B12" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -8571,16 +8612,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="48" t="str">
+      <c r="B21" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -8736,16 +8777,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="48" t="str">
+      <c r="B30" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="50"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -8904,16 +8945,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="48" t="str">
+      <c r="B39" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="50"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -9057,16 +9098,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="48" t="str">
+      <c r="B48" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -9226,16 +9267,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="48" t="str">
+      <c r="B57" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="50"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="48"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -9399,16 +9440,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="48" t="str">
+      <c r="B66" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="50"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="48"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -9550,16 +9591,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="48" t="str">
+      <c r="B75" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="50"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -9701,16 +9742,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="48" t="str">
+      <c r="B84" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
-      <c r="H84" s="50"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="48"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -9849,17 +9890,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9870,11 +9911,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95CCB1C-9FB8-4566-AB28-8B8BAEC7F6E6}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -10139,32 +10180,32 @@
         <f>Total!$G$1</f>
         <v>Week 3</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -10335,16 +10376,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="48" t="str">
+      <c r="B12" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -10508,16 +10549,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="48" t="str">
+      <c r="B21" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -10657,16 +10698,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="48" t="str">
+      <c r="B30" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="50"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -10820,16 +10861,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="48" t="str">
+      <c r="B39" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="50"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -10995,16 +11036,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="48" t="str">
+      <c r="B48" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -11161,16 +11202,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="48" t="str">
+      <c r="B57" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="50"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="48"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -11324,16 +11365,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="48" t="str">
+      <c r="B66" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="50"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="48"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -11475,16 +11516,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="48" t="str">
+      <c r="B75" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="50"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -11626,16 +11667,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="48" t="str">
+      <c r="B84" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
-      <c r="H84" s="50"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="48"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -11774,17 +11815,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11795,11 +11836,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB66144-3102-4D48-A4D0-FA37996B20EF}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -12064,32 +12105,32 @@
         <f>Total!$H$1</f>
         <v>Week 4</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -12272,16 +12313,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B13" s="48" t="str">
+      <c r="B13" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="str">
@@ -12443,16 +12484,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B22" s="48" t="str">
+      <c r="B22" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="str">
@@ -12592,16 +12633,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B31" s="48" t="str">
+      <c r="B31" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="50"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="48"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="str">
@@ -12763,16 +12804,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B40" s="48" t="str">
+      <c r="B40" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="50"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="48"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="str">
@@ -12938,16 +12979,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B49" s="48" t="str">
+      <c r="B49" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="50"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="48"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="str">
@@ -13107,16 +13148,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B58" s="48" t="str">
+      <c r="B58" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="50"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="48"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="str">
@@ -13154,56 +13195,70 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
+      <c r="C60" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="6">
         <f>SUM(B60:G60)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
+      <c r="A61" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
+      <c r="E61" s="10">
+        <v>2.5</v>
+      </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="6">
         <f t="shared" ref="H61:H64" si="15">SUM(B61:G61)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="9"/>
+      <c r="A62" s="9" t="s">
+        <v>165</v>
+      </c>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
+      <c r="F62" s="10">
+        <v>2</v>
+      </c>
       <c r="G62" s="10"/>
       <c r="H62" s="6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
+      <c r="A63" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
+      <c r="G63" s="10">
+        <v>3</v>
+      </c>
       <c r="H63" s="6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -13230,7 +13285,7 @@
       </c>
       <c r="C65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D65" s="11">
         <f t="shared" si="16"/>
@@ -13238,19 +13293,19 @@
       </c>
       <c r="E65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H65" s="11">
         <f>SUM(B65:G65)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
@@ -13258,16 +13313,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B67" s="48" t="str">
+      <c r="B67" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="50"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="48"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="str">
@@ -13409,16 +13464,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B76" s="48" t="str">
+      <c r="B76" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="49"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="49"/>
-      <c r="H76" s="50"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="48"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="str">
@@ -13560,16 +13615,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B85" s="48" t="str">
+      <c r="B85" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C85" s="49"/>
-      <c r="D85" s="49"/>
-      <c r="E85" s="49"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="49"/>
-      <c r="H85" s="50"/>
+      <c r="C85" s="47"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="47"/>
+      <c r="G85" s="47"/>
+      <c r="H85" s="48"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="str">
@@ -13708,17 +13763,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B31:H31"/>
     <mergeCell ref="B85:H85"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B58:H58"/>
     <mergeCell ref="B67:H67"/>
     <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13729,11 +13784,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876A7822-F1F7-440D-86F1-601DBA89356E}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -13998,31 +14053,31 @@
         <f>Total!$I$1</f>
         <v>Week 5</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -14179,16 +14234,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B11" s="48" t="str">
+      <c r="B11" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="50"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="48"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="str">
@@ -14354,16 +14409,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B20" s="48" t="str">
+      <c r="B20" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="str">
@@ -14503,16 +14558,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B29" s="48" t="str">
+      <c r="B29" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="50"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="48"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="str">
@@ -14670,16 +14725,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B38" s="48" t="str">
+      <c r="B38" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="50"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="48"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="str">
@@ -14835,16 +14890,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B47" s="48" t="str">
+      <c r="B47" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="50"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="48"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="str">
@@ -15002,16 +15057,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B56" s="48" t="str">
+      <c r="B56" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="50"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="48"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="str">
@@ -15049,30 +15104,36 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
+      <c r="C58" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="6">
         <f>SUM(B58:G58)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="9"/>
+      <c r="A59" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
+      <c r="E59" s="10">
+        <v>2.5</v>
+      </c>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="6">
         <f t="shared" ref="H59:H62" si="15">SUM(B59:G59)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -15125,7 +15186,7 @@
       </c>
       <c r="C63" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D63" s="11">
         <f t="shared" si="16"/>
@@ -15133,7 +15194,7 @@
       </c>
       <c r="E63" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F63" s="11">
         <f t="shared" si="16"/>
@@ -15145,7 +15206,7 @@
       </c>
       <c r="H63" s="11">
         <f>SUM(B63:G63)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
@@ -15153,16 +15214,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B65" s="48" t="str">
+      <c r="B65" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="50"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="48"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="str">
@@ -15304,16 +15365,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B74" s="48" t="str">
+      <c r="B74" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="49"/>
-      <c r="G74" s="49"/>
-      <c r="H74" s="50"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="47"/>
+      <c r="H74" s="48"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="str">
@@ -15455,16 +15516,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B83" s="48" t="str">
+      <c r="B83" s="46" t="str">
         <f>$B$3</f>
         <v>Uren</v>
       </c>
-      <c r="C83" s="49"/>
-      <c r="D83" s="49"/>
-      <c r="E83" s="49"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="49"/>
-      <c r="H83" s="50"/>
+      <c r="C83" s="47"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="47"/>
+      <c r="H83" s="48"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="str">
@@ -15603,17 +15664,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B29:H29"/>
     <mergeCell ref="B83:H83"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="B47:H47"/>
     <mergeCell ref="B56:H56"/>
     <mergeCell ref="B65:H65"/>
     <mergeCell ref="B74:H74"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B29:H29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15624,11 +15685,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD24EE9A-1C5D-4003-B9D2-5E40317F9E20}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -15893,32 +15954,32 @@
         <f>Total!$J$1</f>
         <v>Week 6</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -16108,16 +16169,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B13" s="48" t="str">
+      <c r="B13" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="50"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="str">
@@ -16281,16 +16342,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B22" s="48" t="str">
+      <c r="B22" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="str">
@@ -16430,16 +16491,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B31" s="48" t="str">
+      <c r="B31" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="50"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="48"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="str">
@@ -16605,16 +16666,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B40" s="48" t="str">
+      <c r="B40" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="50"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="48"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="str">
@@ -16771,16 +16832,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B49" s="48" t="str">
+      <c r="B49" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="50"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="48"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="str">
@@ -16940,16 +17001,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B58" s="48" t="str">
+      <c r="B58" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="50"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="48"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="str">
@@ -16987,69 +17048,89 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
+      <c r="C60" s="10">
+        <v>2.5</v>
+      </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="6">
         <f>SUM(B60:G60)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
+      <c r="A61" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
+      <c r="E61" s="10">
+        <v>2.5</v>
+      </c>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="6">
         <f t="shared" ref="H61:H64" si="15">SUM(B61:G61)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="9"/>
+      <c r="A62" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
+      <c r="F62" s="10">
+        <v>2</v>
+      </c>
       <c r="G62" s="10"/>
       <c r="H62" s="6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
+      <c r="A63" s="9" t="s">
+        <v>167</v>
+      </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
+      <c r="G63" s="10">
+        <v>4</v>
+      </c>
       <c r="H63" s="6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
+      <c r="A64" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="10">
+        <v>3</v>
+      </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
+      <c r="E64" s="10">
+        <v>1</v>
+      </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="6">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -17059,11 +17140,11 @@
       </c>
       <c r="B65" s="11">
         <f t="shared" ref="B65:G65" si="16">SUM(B60:B64)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D65" s="11">
         <f t="shared" si="16"/>
@@ -17071,19 +17152,19 @@
       </c>
       <c r="E65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G65" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H65" s="11">
         <f>SUM(B65:G65)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
@@ -17091,16 +17172,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B67" s="48" t="str">
+      <c r="B67" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="50"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="48"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="str">
@@ -17242,16 +17323,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B76" s="48" t="str">
+      <c r="B76" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-      <c r="E76" s="49"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="49"/>
-      <c r="H76" s="50"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="48"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="str">
@@ -17393,16 +17474,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B85" s="48" t="str">
+      <c r="B85" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C85" s="49"/>
-      <c r="D85" s="49"/>
-      <c r="E85" s="49"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="49"/>
-      <c r="H85" s="50"/>
+      <c r="C85" s="47"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="47"/>
+      <c r="G85" s="47"/>
+      <c r="H85" s="48"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="str">
@@ -17541,17 +17622,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B31:H31"/>
     <mergeCell ref="B85:H85"/>
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B58:H58"/>
     <mergeCell ref="B67:H67"/>
     <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17562,11 +17643,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0BDF61-7E89-4C92-A82D-1FF14F8FEE71}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.42578125" style="5" customWidth="1"/>
     <col min="2" max="7" width="7.140625" style="5" customWidth="1"/>
@@ -17831,32 +17912,32 @@
         <f>Total!$K$1</f>
         <v>Week 7</v>
       </c>
-      <c r="B1" s="46" t="str">
+      <c r="B1" s="49" t="str">
         <f>'Week (1)'!$B$1</f>
         <v>Uren TOTAAL</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="str">
         <f>Total!D2</f>
         <v>Jafar Alirahmi</v>
       </c>
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="46" t="str">
         <f>'Week (1)'!$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="50"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
@@ -18006,16 +18087,16 @@
         <f>Total!D3</f>
         <v>Viktor Krastev</v>
       </c>
-      <c r="B12" s="48" t="str">
+      <c r="B12" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
@@ -18187,16 +18268,16 @@
         <f>Total!D4</f>
         <v>Justin Fuchs</v>
       </c>
-      <c r="B21" s="48" t="str">
+      <c r="B21" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
@@ -18336,16 +18417,16 @@
         <f>Total!D5</f>
         <v>Rubén Gómez</v>
       </c>
-      <c r="B30" s="48" t="str">
+      <c r="B30" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="50"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
@@ -18511,16 +18592,16 @@
         <f>Total!D6</f>
         <v>Yaroslav Peptiuk</v>
       </c>
-      <c r="B39" s="48" t="str">
+      <c r="B39" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="50"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
@@ -18662,16 +18743,16 @@
         <f>Total!D7</f>
         <v>Aleks Proskurkin</v>
       </c>
-      <c r="B48" s="48" t="str">
+      <c r="B48" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
@@ -18831,16 +18912,16 @@
         <f>Total!D8</f>
         <v>Ferhat Kelten</v>
       </c>
-      <c r="B57" s="48" t="str">
+      <c r="B57" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="50"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="48"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="str">
@@ -18878,17 +18959,19 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
+      <c r="F59" s="10">
+        <v>1</v>
+      </c>
       <c r="G59" s="10"/>
       <c r="H59" s="6">
         <f>SUM(B59:G59)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -18966,7 +19049,7 @@
       </c>
       <c r="F64" s="11">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="11">
         <f t="shared" si="16"/>
@@ -18974,7 +19057,7 @@
       </c>
       <c r="H64" s="11">
         <f>SUM(B64:G64)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
@@ -18982,16 +19065,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B66" s="48" t="str">
+      <c r="B66" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="50"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="48"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
@@ -19133,16 +19216,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B75" s="48" t="str">
+      <c r="B75" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="50"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="48"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
@@ -19284,16 +19367,16 @@
         <f>Total!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B84" s="48" t="str">
+      <c r="B84" s="46" t="str">
         <f>$B$3</f>
         <v>Hours</v>
       </c>
-      <c r="C84" s="49"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
-      <c r="H84" s="50"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="48"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
@@ -19432,17 +19515,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="B84:H84"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B66:H66"/>
     <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19450,6 +19533,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </c6664f9864b54a78bdf9e6230de1c78b>
+    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100294690D6A57C3C4B8650464765815F1C" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="bf1d2ff51e740e451b46e7c13bf9e6da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45f6ce90-ba85-4ef2-b43f-c64448cd95eb" xmlns:ns3="c7549584-aa9c-449c-abfe-2ca02f3a7188" xmlns:ns4="6c73e52c-07d4-4617-ab67-464747257e8d" xmlns:ns5="ab37b2fe-4f81-426e-b942-40459dbac68c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8575fd65d7959dd12bd4dc11d36e634e" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="45f6ce90-ba85-4ef2-b43f-c64448cd95eb"/>
@@ -19692,27 +19795,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <c6664f9864b54a78bdf9e6230de1c78b xmlns="6c73e52c-07d4-4617-ab67-464747257e8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </c6664f9864b54a78bdf9e6230de1c78b>
-    <Versiebeheer xmlns="ab37b2fe-4f81-426e-b942-40459dbac68c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
+    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{724CCB8E-5E6A-4B8C-A558-5D9223ADF390}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19731,23 +19833,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477D1558-F7E0-401F-8472-E1151A96BE17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6c73e52c-07d4-4617-ab67-464747257e8d"/>
-    <ds:schemaRef ds:uri="ab37b2fe-4f81-426e-b942-40459dbac68c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{844B94A5-2CB8-4D3A-A97F-85854BBCA257}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>